<commit_message>
Add password to LOGIN_USER
</commit_message>
<xml_diff>
--- a/DATA DICTIONARY/DATA DICTIONARY.xlsx
+++ b/DATA DICTIONARY/DATA DICTIONARY.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
   <si>
     <t>Contents</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Login User</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -628,8 +631,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,8 +716,8 @@
   </sheetPr>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,13 +834,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1024</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -847,16 +853,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -866,16 +869,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="10">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -886,16 +889,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="10">
+        <v>50</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -905,21 +908,36 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="10">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -1276,10 +1294,10 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C13 C18:C111">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C111 C3:C13">
       <formula1>"VARCHAR2,NUMBER,INTEGER,DATE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H98 E3:E13 E18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H98 E18 E3:E13">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>